<commit_message>
all data is read as seperate dicts
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10B840-9B45-4450-ACE0-081A27D7AA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F390AE-FC48-48FE-85FA-027201EA3B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="5" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>K10</t>
+  </si>
+  <si>
+    <t>fuel cost</t>
+  </si>
+  <si>
+    <t>labor cost</t>
   </si>
 </sst>
 </file>
@@ -1106,15 +1112,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1127,8 +1133,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1141,8 +1150,11 @@
       <c r="D2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1155,8 +1167,11 @@
       <c r="D3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1169,8 +1184,11 @@
       <c r="D4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1183,8 +1201,11 @@
       <c r="D5">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1197,8 +1218,11 @@
       <c r="D6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1211,8 +1235,11 @@
       <c r="D7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1225,8 +1252,11 @@
       <c r="D8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1239,8 +1269,11 @@
       <c r="D9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1253,8 +1286,11 @@
       <c r="D10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1266,6 +1302,9 @@
       </c>
       <c r="D11">
         <v>1000</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1326,7 +1365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3AA453-9DF3-487A-B6B1-8F8E8CA072C9}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1369,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A52EF1-80D4-47B1-A5FA-9BC1590D36D2}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1420,6 +1459,14 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all constraints and simple visualization of solution added
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Masterthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F390AE-FC48-48FE-85FA-027201EA3B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAE285C-5159-46C4-A76E-0095A808B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Nodes" sheetId="2" r:id="rId2"/>
-    <sheet name="Products" sheetId="3" r:id="rId3"/>
-    <sheet name="Trucks" sheetId="4" r:id="rId4"/>
+    <sheet name="Trucks" sheetId="4" r:id="rId3"/>
+    <sheet name="Products" sheetId="3" r:id="rId4"/>
     <sheet name="Depots" sheetId="6" r:id="rId5"/>
     <sheet name="Sizes" sheetId="7" r:id="rId6"/>
     <sheet name="Others" sheetId="5" r:id="rId7"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -141,36 +141,6 @@
   </si>
   <si>
     <t>N10</t>
-  </si>
-  <si>
-    <t>N11</t>
-  </si>
-  <si>
-    <t>N12</t>
-  </si>
-  <si>
-    <t>N13</t>
-  </si>
-  <si>
-    <t>N14</t>
-  </si>
-  <si>
-    <t>N15</t>
-  </si>
-  <si>
-    <t>N16</t>
-  </si>
-  <si>
-    <t>N17</t>
-  </si>
-  <si>
-    <t>N18</t>
-  </si>
-  <si>
-    <t>N19</t>
-  </si>
-  <si>
-    <t>N20</t>
   </si>
   <si>
     <t>0;0</t>
@@ -584,13 +554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DA4CFF-849F-402D-A31E-36AFD7D9F3E3}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -618,13 +588,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -635,13 +605,13 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E3">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -652,13 +622,13 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -669,13 +639,13 @@
         <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -686,10 +656,10 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E6">
-        <v>33</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -700,15 +670,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E7E8C8-2BBC-4DCF-8CDF-FCF7EA07A2CA}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -736,13 +706,13 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -753,13 +723,13 @@
         <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -770,13 +740,13 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -787,13 +757,13 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -804,13 +774,13 @@
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -821,13 +791,13 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -838,13 +808,13 @@
         <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -855,13 +825,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -872,13 +842,13 @@
         <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -889,179 +859,9 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14">
-        <v>67</v>
-      </c>
-      <c r="C14">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15">
-        <v>82</v>
-      </c>
-      <c r="C15">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16">
-        <v>40</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17">
-        <v>93</v>
-      </c>
-      <c r="C17">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18">
-        <v>61</v>
-      </c>
-      <c r="C18">
-        <v>68</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20">
-        <v>15</v>
-      </c>
-      <c r="C20">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21">
-        <v>52</v>
-      </c>
-      <c r="C21">
-        <v>86</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21">
         <v>0</v>
       </c>
     </row>
@@ -1072,243 +872,243 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF51854-3197-4240-AE12-300BE0937092}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3">
+        <v>100000</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>100000</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6">
+        <v>100000</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>100000</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>100000</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>100000</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>150</v>
+      </c>
+      <c r="D10">
+        <v>100000</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <v>100000</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF51854-3197-4240-AE12-300BE0937092}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2">
-        <v>90</v>
-      </c>
-      <c r="C2">
-        <v>150</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3">
-        <v>90</v>
-      </c>
-      <c r="C3">
-        <v>150</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4">
-        <v>90</v>
-      </c>
-      <c r="C4">
-        <v>150</v>
-      </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5">
-        <v>90</v>
-      </c>
-      <c r="C5">
-        <v>150</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6">
-        <v>90</v>
-      </c>
-      <c r="C6">
-        <v>150</v>
-      </c>
-      <c r="D6">
-        <v>1000</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7">
-        <v>90</v>
-      </c>
-      <c r="C7">
-        <v>150</v>
-      </c>
-      <c r="D7">
-        <v>1000</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8">
-        <v>90</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8">
-        <v>1000</v>
-      </c>
-      <c r="E8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9">
-        <v>90</v>
-      </c>
-      <c r="C9">
-        <v>150</v>
-      </c>
-      <c r="D9">
-        <v>1000</v>
-      </c>
-      <c r="E9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10">
-        <v>90</v>
-      </c>
-      <c r="C10">
-        <v>150</v>
-      </c>
-      <c r="D10">
-        <v>1000</v>
-      </c>
-      <c r="E10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11">
-        <v>90</v>
-      </c>
-      <c r="C11">
-        <v>150</v>
-      </c>
-      <c r="D11">
-        <v>1000</v>
-      </c>
-      <c r="E11">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1318,12 +1118,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1345,7 +1145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1366,37 +1166,37 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1410,16 +1210,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A52EF1-80D4-47B1-A5FA-9BC1590D36D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1427,41 +1227,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>25</v>

</xml_diff>

<commit_message>
callback method added (no updating constraints yet)
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAE285C-5159-46C4-A76E-0095A808B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AA06A6-C55B-459F-AC92-388233E42951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Depots" sheetId="6" r:id="rId5"/>
     <sheet name="Sizes" sheetId="7" r:id="rId6"/>
     <sheet name="Others" sheetId="5" r:id="rId7"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -554,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DA4CFF-849F-402D-A31E-36AFD7D9F3E3}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H6:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +674,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +910,7 @@
         <v>150</v>
       </c>
       <c r="D2">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E2">
         <v>12</v>
@@ -926,7 +927,7 @@
         <v>150</v>
       </c>
       <c r="D3">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -943,7 +944,7 @@
         <v>150</v>
       </c>
       <c r="D4">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E4">
         <v>12</v>
@@ -960,7 +961,7 @@
         <v>150</v>
       </c>
       <c r="D5">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -977,7 +978,7 @@
         <v>150</v>
       </c>
       <c r="D6">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -994,7 +995,7 @@
         <v>150</v>
       </c>
       <c r="D7">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -1011,7 +1012,7 @@
         <v>150</v>
       </c>
       <c r="D8">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1028,7 +1029,7 @@
         <v>150</v>
       </c>
       <c r="D9">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E9">
         <v>12</v>
@@ -1045,7 +1046,7 @@
         <v>150</v>
       </c>
       <c r="D10">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E10">
         <v>12</v>
@@ -1062,7 +1063,7 @@
         <v>150</v>
       </c>
       <c r="D11">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="E11">
         <v>12</v>
@@ -1211,7 +1212,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E1" sqref="E1:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,4 +1271,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFEA688-AA57-46FF-A88A-ED5634412B20}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lazy contraints added in model
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Masterthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AA06A6-C55B-459F-AC92-388233E42951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422051E9-D536-49EA-B716-3BEDA343CB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -559,9 +559,9 @@
       <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -595,7 +595,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -612,7 +612,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -629,7 +629,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -646,7 +646,7 @@
         <v>0.36666666666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -673,13 +673,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E7E8C8-2BBC-4DCF-8CDF-FCF7EA07A2CA}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -876,13 +876,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -916,7 +916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -933,7 +933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -950,7 +950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -967,7 +967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -984,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1083,9 +1083,9 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1122,9 +1122,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1170,34 +1170,34 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1215,12 +1215,12 @@
       <selection activeCell="E1" sqref="E1:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1278,10 +1278,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="E9" sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
number of arcs limited.
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Masterthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422051E9-D536-49EA-B716-3BEDA343CB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7F0DDD-056C-416C-BB3A-E4583C385CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Nodes" sheetId="2" r:id="rId2"/>
-    <sheet name="Trucks" sheetId="4" r:id="rId3"/>
-    <sheet name="Products" sheetId="3" r:id="rId4"/>
-    <sheet name="Depots" sheetId="6" r:id="rId5"/>
-    <sheet name="Sizes" sheetId="7" r:id="rId6"/>
-    <sheet name="Others" sheetId="5" r:id="rId7"/>
-    <sheet name="Tabelle1" sheetId="8" r:id="rId8"/>
+    <sheet name="Depots" sheetId="6" r:id="rId3"/>
+    <sheet name="Alle" sheetId="9" r:id="rId4"/>
+    <sheet name="Trucks" sheetId="4" r:id="rId5"/>
+    <sheet name="Products" sheetId="3" r:id="rId6"/>
+    <sheet name="Sizes" sheetId="7" r:id="rId7"/>
+    <sheet name="Others" sheetId="5" r:id="rId8"/>
+    <sheet name="Distances" sheetId="8" r:id="rId9"/>
+    <sheet name="Arcs" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -196,6 +198,12 @@
   </si>
   <si>
     <t>labor cost</t>
+  </si>
+  <si>
+    <t>WENN(UND(Distances!B2&lt;Arcs!$S$1;Distances!B2&gt;0);1;0)</t>
+  </si>
+  <si>
+    <t>Node</t>
   </si>
 </sst>
 </file>
@@ -556,12 +564,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -595,7 +603,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -612,7 +620,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -629,7 +637,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -646,7 +654,7 @@
         <v>0.36666666666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -665,6 +673,1103 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C86A240-AD32-4D4E-ACE7-7D6C73E98EA7}">
+  <dimension ref="A1:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>SUM(B2:R2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S18" si="0">SUM(B3:R3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -673,13 +1778,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E7E8C8-2BBC-4DCF-8CDF-FCF7EA07A2CA}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -713,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -730,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -747,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -764,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -781,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -798,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -815,12 +1920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -832,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -849,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -873,6 +1978,256 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFE4162-6F2B-4130-A7E9-BB2F55C3BC68}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C05BCD-EC1D-45AF-AD56-889E417747D3}">
+  <dimension ref="A2:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>64</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>98</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CB4B-AC88-4BE8-99F7-55E14605BA85}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -880,9 +2235,9 @@
       <selection activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +2254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -916,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -933,7 +2288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -950,7 +2305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -967,7 +2322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -984,7 +2339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1001,7 +2356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1018,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1035,7 +2390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1052,7 +2407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1075,7 +2430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF51854-3197-4240-AE12-300BE0937092}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1083,9 +2438,9 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1101,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1114,55 +2469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFE4162-6F2B-4130-A7E9-BB2F55C3BC68}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>77</v>
-      </c>
-      <c r="C2">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3AA453-9DF3-487A-B6B1-8F8E8CA072C9}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -1170,34 +2477,34 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1207,7 +2514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A52EF1-80D4-47B1-A5FA-9BC1590D36D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1215,12 +2522,12 @@
       <selection activeCell="E1" sqref="E1:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1228,7 +2535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +2543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +2559,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1260,7 +2567,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1273,16 +2580,1307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFEA688-AA57-46FF-A88A-ED5634412B20}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:E9"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.591808301161009</v>
+      </c>
+      <c r="D2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.188234163113421</v>
+      </c>
+      <c r="E2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>74.249579123386283</v>
+      </c>
+      <c r="F2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.154759474226502</v>
+      </c>
+      <c r="G2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>115.27792503337315</v>
+      </c>
+      <c r="H2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>102.08329931972223</v>
+      </c>
+      <c r="I2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>67.623960250786851</v>
+      </c>
+      <c r="J2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>28.600699292150182</v>
+      </c>
+      <c r="K2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>81.024687595818591</v>
+      </c>
+      <c r="L2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>50.24937810560445</v>
+      </c>
+      <c r="M2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.201108024738787</v>
+      </c>
+      <c r="N2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>38.013155617496423</v>
+      </c>
+      <c r="O2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>46.529560496527367</v>
+      </c>
+      <c r="P2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.529964086141668</v>
+      </c>
+      <c r="Q2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>86.452298986203942</v>
+      </c>
+      <c r="R2">
+        <f>SQRT((VLOOKUP($A2,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A2,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.345009313209601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.591808301161009</v>
+      </c>
+      <c r="C3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.006944109578768</v>
+      </c>
+      <c r="E3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>49.040799340956916</v>
+      </c>
+      <c r="G3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.400325732035007</v>
+      </c>
+      <c r="H3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>44.045431091090478</v>
+      </c>
+      <c r="I3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.011626335213137</v>
+      </c>
+      <c r="J3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.227829907617071</v>
+      </c>
+      <c r="K3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.413111231467404</v>
+      </c>
+      <c r="L3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.465437442517235</v>
+      </c>
+      <c r="M3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>14.142135623730951</v>
+      </c>
+      <c r="N3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.529646120466801</v>
+      </c>
+      <c r="O3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>48.846698967279252</v>
+      </c>
+      <c r="P3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.630789467763066</v>
+      </c>
+      <c r="Q3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>32.695565448543633</v>
+      </c>
+      <c r="R3">
+        <f>SQRT((VLOOKUP($A3,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A3,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>16.643316977093239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.188234163113421</v>
+      </c>
+      <c r="C4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.006944109578768</v>
+      </c>
+      <c r="D4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>64.381674411279491</v>
+      </c>
+      <c r="F4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.438350715445125</v>
+      </c>
+      <c r="G4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>97.082439194738001</v>
+      </c>
+      <c r="H4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>98.127468121826112</v>
+      </c>
+      <c r="I4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>39.05124837953327</v>
+      </c>
+      <c r="J4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.010637094172637</v>
+      </c>
+      <c r="K4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>79.075912893876861</v>
+      </c>
+      <c r="L4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.206555615733702</v>
+      </c>
+      <c r="M4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.491935064237495</v>
+      </c>
+      <c r="N4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.336925203941234</v>
+      </c>
+      <c r="O4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>23.600847442411894</v>
+      </c>
+      <c r="P4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>69.892775020026207</v>
+      </c>
+      <c r="Q4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.058419397233934</v>
+      </c>
+      <c r="R4">
+        <f>SQRT((VLOOKUP($A4,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A4,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>55.461698495448189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>74.249579123386283</v>
+      </c>
+      <c r="C5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>64.381674411279491</v>
+      </c>
+      <c r="E5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.561891462814962</v>
+      </c>
+      <c r="G5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>41.109609582188931</v>
+      </c>
+      <c r="H5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.058772731852805</v>
+      </c>
+      <c r="I5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>26.570660511172846</v>
+      </c>
+      <c r="J5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>46.097722286464439</v>
+      </c>
+      <c r="K5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>15.231546211727817</v>
+      </c>
+      <c r="L5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>57.078892771321343</v>
+      </c>
+      <c r="M5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>18.867962264113206</v>
+      </c>
+      <c r="N5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>53.851648071345039</v>
+      </c>
+      <c r="O5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>45.541190146942803</v>
+      </c>
+      <c r="P5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>71.847059786744225</v>
+      </c>
+      <c r="Q5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>13.601470508735444</v>
+      </c>
+      <c r="R5">
+        <f>SQRT((VLOOKUP($A5,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A5,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>22.022715545545239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.154759474226502</v>
+      </c>
+      <c r="C6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>49.040799340956916</v>
+      </c>
+      <c r="D6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.438350715445125</v>
+      </c>
+      <c r="E6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.561891462814962</v>
+      </c>
+      <c r="F6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>94.873600121424715</v>
+      </c>
+      <c r="H6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>86.977008456258133</v>
+      </c>
+      <c r="I6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>40.80441152620633</v>
+      </c>
+      <c r="J6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>15.231546211727817</v>
+      </c>
+      <c r="K6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>65.520989003524662</v>
+      </c>
+      <c r="L6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>22.472205054244231</v>
+      </c>
+      <c r="M6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.539902586416787</v>
+      </c>
+      <c r="N6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>44.82186966202994</v>
+      </c>
+      <c r="O6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>17.464249196572979</v>
+      </c>
+      <c r="P6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.902646142032481</v>
+      </c>
+      <c r="Q6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>68.029405406779802</v>
+      </c>
+      <c r="R6">
+        <f>SQRT((VLOOKUP($A6,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A6,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.693136595149497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>115.27792503337315</v>
+      </c>
+      <c r="C7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.400325732035007</v>
+      </c>
+      <c r="D7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>97.082439194738001</v>
+      </c>
+      <c r="E7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>41.109609582188931</v>
+      </c>
+      <c r="F7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>94.873600121424715</v>
+      </c>
+      <c r="G7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.179356624028344</v>
+      </c>
+      <c r="I7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.821764679410968</v>
+      </c>
+      <c r="J7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>87.206651122491792</v>
+      </c>
+      <c r="K7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>37.12142238654117</v>
+      </c>
+      <c r="L7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>92.973114393355672</v>
+      </c>
+      <c r="M7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.853944456021594</v>
+      </c>
+      <c r="N7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>90.917545061445651</v>
+      </c>
+      <c r="O7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>83.258633185994597</v>
+      </c>
+      <c r="P7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>112.16059914247963</v>
+      </c>
+      <c r="Q7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.206163733020468</v>
+      </c>
+      <c r="R7">
+        <f>SQRT((VLOOKUP($A7,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A7,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>62.936475910238251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>102.08329931972223</v>
+      </c>
+      <c r="C8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>44.045431091090478</v>
+      </c>
+      <c r="D8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>98.127468121826112</v>
+      </c>
+      <c r="E8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.058772731852805</v>
+      </c>
+      <c r="F8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>86.977008456258133</v>
+      </c>
+      <c r="G8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.179356624028344</v>
+      </c>
+      <c r="H8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.413803110051795</v>
+      </c>
+      <c r="J8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>76.05918747922567</v>
+      </c>
+      <c r="K8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>21.540659228538015</v>
+      </c>
+      <c r="L8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>91.13725912051558</v>
+      </c>
+      <c r="M8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30</v>
+      </c>
+      <c r="N8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.249567472753768</v>
+      </c>
+      <c r="O8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>79.511005527536881</v>
+      </c>
+      <c r="P8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>96.674712308855618</v>
+      </c>
+      <c r="Q8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>21.095023109728988</v>
+      </c>
+      <c r="R8">
+        <f>SQRT((VLOOKUP($A8,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A8,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>51.623637996561229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>67.623960250786851</v>
+      </c>
+      <c r="C9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.011626335213137</v>
+      </c>
+      <c r="D9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>39.05124837953327</v>
+      </c>
+      <c r="E9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>26.570660511172846</v>
+      </c>
+      <c r="F9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>40.80441152620633</v>
+      </c>
+      <c r="G9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.821764679410968</v>
+      </c>
+      <c r="H9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.413803110051795</v>
+      </c>
+      <c r="I9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>40.26164427839479</v>
+      </c>
+      <c r="K9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>41.785164831552358</v>
+      </c>
+      <c r="L9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.176014981270121</v>
+      </c>
+      <c r="M9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.011626335213137</v>
+      </c>
+      <c r="N9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.98386886924694</v>
+      </c>
+      <c r="O9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.612496949731394</v>
+      </c>
+      <c r="P9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>69.856996786291916</v>
+      </c>
+      <c r="Q9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>38.327535793473601</v>
+      </c>
+      <c r="R9">
+        <f>SQRT((VLOOKUP($A9,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A9,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>28.231188426986208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>28.600699292150182</v>
+      </c>
+      <c r="C10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.227829907617071</v>
+      </c>
+      <c r="D10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.010637094172637</v>
+      </c>
+      <c r="E10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>46.097722286464439</v>
+      </c>
+      <c r="F10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>15.231546211727817</v>
+      </c>
+      <c r="G10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>87.206651122491792</v>
+      </c>
+      <c r="H10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>76.05918747922567</v>
+      </c>
+      <c r="I10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>40.26164427839479</v>
+      </c>
+      <c r="J10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.561891462814962</v>
+      </c>
+      <c r="L10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.828149534535996</v>
+      </c>
+      <c r="M10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.127486671792717</v>
+      </c>
+      <c r="N10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30.413812651491099</v>
+      </c>
+      <c r="O10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.079872407968907</v>
+      </c>
+      <c r="P10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.614185789921695</v>
+      </c>
+      <c r="Q10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.821764679410968</v>
+      </c>
+      <c r="R10">
+        <f>SQRT((VLOOKUP($A10,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A10,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.698178070456937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>81.024687595818591</v>
+      </c>
+      <c r="C11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.413111231467404</v>
+      </c>
+      <c r="D11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>79.075912893876861</v>
+      </c>
+      <c r="E11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>15.231546211727817</v>
+      </c>
+      <c r="F11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>65.520989003524662</v>
+      </c>
+      <c r="G11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>37.12142238654117</v>
+      </c>
+      <c r="H11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>21.540659228538015</v>
+      </c>
+      <c r="I11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>41.785164831552358</v>
+      </c>
+      <c r="J11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.561891462814962</v>
+      </c>
+      <c r="K11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>71.06335201775947</v>
+      </c>
+      <c r="M11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>10.770329614269007</v>
+      </c>
+      <c r="N11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>53.851648071345039</v>
+      </c>
+      <c r="O11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.008473967727717</v>
+      </c>
+      <c r="P11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>76.380625815713245</v>
+      </c>
+      <c r="Q11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>10.04987562112089</v>
+      </c>
+      <c r="R11">
+        <f>SQRT((VLOOKUP($A11,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A11,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30.083217912982647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>50.24937810560445</v>
+      </c>
+      <c r="C12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.465437442517235</v>
+      </c>
+      <c r="D12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.206555615733702</v>
+      </c>
+      <c r="E12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>57.078892771321343</v>
+      </c>
+      <c r="F12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>22.472205054244231</v>
+      </c>
+      <c r="G12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>92.973114393355672</v>
+      </c>
+      <c r="H12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>91.13725912051558</v>
+      </c>
+      <c r="I12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.176014981270121</v>
+      </c>
+      <c r="J12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>34.828149534535996</v>
+      </c>
+      <c r="K12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>71.06335201775947</v>
+      </c>
+      <c r="L12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>68.249542123006222</v>
+      </c>
+      <c r="N12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>65.192024052026483</v>
+      </c>
+      <c r="O12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.649110640673518</v>
+      </c>
+      <c r="P12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.240879114244144</v>
+      </c>
+      <c r="Q12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>70.34912934784623</v>
+      </c>
+      <c r="R12">
+        <f>SQRT((VLOOKUP($A12,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A12,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>45.221676218380054</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.201108024738787</v>
+      </c>
+      <c r="C13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>14.142135623730951</v>
+      </c>
+      <c r="D13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.491935064237495</v>
+      </c>
+      <c r="E13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>18.867962264113206</v>
+      </c>
+      <c r="F13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.539902586416787</v>
+      </c>
+      <c r="G13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.853944456021594</v>
+      </c>
+      <c r="H13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.011626335213137</v>
+      </c>
+      <c r="J13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>47.127486671792717</v>
+      </c>
+      <c r="K13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>10.770329614269007</v>
+      </c>
+      <c r="L13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>68.249542123006222</v>
+      </c>
+      <c r="M13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.266615305567875</v>
+      </c>
+      <c r="O13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>55.731499172371095</v>
+      </c>
+      <c r="P13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>66.708320320631671</v>
+      </c>
+      <c r="Q13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="R13">
+        <f>SQRT((VLOOKUP($A13,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A13,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.020824298928627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>38.013155617496423</v>
+      </c>
+      <c r="C14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.529646120466801</v>
+      </c>
+      <c r="D14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.336925203941234</v>
+      </c>
+      <c r="E14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>53.851648071345039</v>
+      </c>
+      <c r="F14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>44.82186966202994</v>
+      </c>
+      <c r="G14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>90.917545061445651</v>
+      </c>
+      <c r="H14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>72.249567472753768</v>
+      </c>
+      <c r="I14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>61.98386886924694</v>
+      </c>
+      <c r="J14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30.413812651491099</v>
+      </c>
+      <c r="K14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>53.851648071345039</v>
+      </c>
+      <c r="L14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>65.192024052026483</v>
+      </c>
+      <c r="M14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>43.266615305567875</v>
+      </c>
+      <c r="N14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.644304369257</v>
+      </c>
+      <c r="P14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>27.892651361962706</v>
+      </c>
+      <c r="Q14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>62.169124169478209</v>
+      </c>
+      <c r="R14">
+        <f>SQRT((VLOOKUP($A14,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A14,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>46.529560496527367</v>
+      </c>
+      <c r="C15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>48.846698967279252</v>
+      </c>
+      <c r="D15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>23.600847442411894</v>
+      </c>
+      <c r="E15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>45.541190146942803</v>
+      </c>
+      <c r="F15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>17.464249196572979</v>
+      </c>
+      <c r="G15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>83.258633185994597</v>
+      </c>
+      <c r="H15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>79.511005527536881</v>
+      </c>
+      <c r="I15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.612496949731394</v>
+      </c>
+      <c r="J15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>25.079872407968907</v>
+      </c>
+      <c r="K15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.008473967727717</v>
+      </c>
+      <c r="L15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.649110640673518</v>
+      </c>
+      <c r="M15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>55.731499172371095</v>
+      </c>
+      <c r="N15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>54.644304369257</v>
+      </c>
+      <c r="O15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.153619241621193</v>
+      </c>
+      <c r="Q15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.033888572581766</v>
+      </c>
+      <c r="R15">
+        <f>SQRT((VLOOKUP($A15,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A15,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>32.572994949804659</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>12.529964086141668</v>
+      </c>
+      <c r="C16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.630789467763066</v>
+      </c>
+      <c r="D16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>69.892775020026207</v>
+      </c>
+      <c r="E16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>71.847059786744225</v>
+      </c>
+      <c r="F16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.902646142032481</v>
+      </c>
+      <c r="G16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>112.16059914247963</v>
+      </c>
+      <c r="H16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>96.674712308855618</v>
+      </c>
+      <c r="I16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>69.856996786291916</v>
+      </c>
+      <c r="J16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.614185789921695</v>
+      </c>
+      <c r="K16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>76.380625815713245</v>
+      </c>
+      <c r="L16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.240879114244144</v>
+      </c>
+      <c r="M16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>66.708320320631671</v>
+      </c>
+      <c r="N16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>27.892651361962706</v>
+      </c>
+      <c r="O16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.153619241621193</v>
+      </c>
+      <c r="P16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(Q$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>82.97590011563598</v>
+      </c>
+      <c r="R16">
+        <f>SQRT((VLOOKUP($A16,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A16,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(R$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>49.929950931279713</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>86.452298986203942</v>
+      </c>
+      <c r="C17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>32.695565448543633</v>
+      </c>
+      <c r="D17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>77.058419397233934</v>
+      </c>
+      <c r="E17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>13.601470508735444</v>
+      </c>
+      <c r="F17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>68.029405406779802</v>
+      </c>
+      <c r="G17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>29.206163733020468</v>
+      </c>
+      <c r="H17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>21.095023109728988</v>
+      </c>
+      <c r="I17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>38.327535793473601</v>
+      </c>
+      <c r="J17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>58.821764679410968</v>
+      </c>
+      <c r="K17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>10.04987562112089</v>
+      </c>
+      <c r="L17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>70.34912934784623</v>
+      </c>
+      <c r="M17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="N17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>62.169124169478209</v>
+      </c>
+      <c r="O17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>59.033888572581766</v>
+      </c>
+      <c r="P17">
+        <f>SQRT((VLOOKUP($A17,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A17,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>82.97590011563598</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(B$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>52.345009313209601</v>
+      </c>
+      <c r="C18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(C$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>16.643316977093239</v>
+      </c>
+      <c r="D18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(D$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>55.461698495448189</v>
+      </c>
+      <c r="E18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(E$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>22.022715545545239</v>
+      </c>
+      <c r="F18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(F$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35.693136595149497</v>
+      </c>
+      <c r="G18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(G$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>62.936475910238251</v>
+      </c>
+      <c r="H18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(H$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>51.623637996561229</v>
+      </c>
+      <c r="I18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(I$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>28.231188426986208</v>
+      </c>
+      <c r="J18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(J$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.698178070456937</v>
+      </c>
+      <c r="K18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(K$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>30.083217912982647</v>
+      </c>
+      <c r="L18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(L$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>45.221676218380054</v>
+      </c>
+      <c r="M18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(M$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>24.020824298928627</v>
+      </c>
+      <c r="N18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(N$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>35</v>
+      </c>
+      <c r="O18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(O$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>32.572994949804659</v>
+      </c>
+      <c r="P18">
+        <f>SQRT((VLOOKUP($A18,Alle!$A$2:$C$18,2,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,2,FALSE))^2 + (VLOOKUP($A18,Alle!$A$2:$C$18,3,FALSE)-VLOOKUP(P$1,Alle!$A$2:$C$18,3,FALSE))^2)</f>
+        <v>49.929950931279713</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new function to read data
</commit_message>
<xml_diff>
--- a/Test_Daten.xlsx
+++ b/Test_Daten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Masterthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7F0DDD-056C-416C-BB3A-E4583C385CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B19D182-7718-4629-AC49-E3E43B08B43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{B435091E-1EE1-4E12-B1BB-7AFADA28837E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -567,9 +567,9 @@
       <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -603,7 +603,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -637,7 +637,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0.36666666666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -685,9 +685,9 @@
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -749,7 +749,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -809,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -869,7 +869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -929,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -989,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1782,9 +1782,9 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1985,9 +1985,9 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2033,9 +2033,9 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2235,9 +2235,9 @@
       <selection activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2438,9 +2438,9 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2477,34 +2477,34 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2522,12 +2522,12 @@
       <selection activeCell="E1" sqref="E1:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2588,9 +2588,9 @@
       <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>52.345009313209601</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>16.643316977093239</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>55.461698495448189</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>22.022715545545239</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>35.693136595149497</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>62.936475910238251</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>51.623637996561229</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>28.231188426986208</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>24.698178070456937</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>30.083217912982647</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>45.221676218380054</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>24.020824298928627</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>32.572994949804659</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>49.929950931279713</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>

</xml_diff>